<commit_message>
I have modified kpp
</commit_message>
<xml_diff>
--- a/kpp.xlsx
+++ b/kpp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP-PC\Desktop\kartik_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA111F1B-E790-40FD-89A7-6AF2F30596A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364609B1-A5B6-460E-8CAD-2A117BFF80CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{587BAC4D-6892-49A0-8656-B3311D4E42E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="5" xr2:uid="{587BAC4D-6892-49A0-8656-B3311D4E42E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice1" sheetId="1" r:id="rId1"/>
@@ -26,17 +26,25 @@
     <definedName name="Employees">Employees!$A$2:$A$6</definedName>
     <definedName name="Location">Location!$A$2:$A$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>First Name</t>
   </si>
@@ -222,6 +230,12 @@
   </si>
   <si>
     <t>Employee Name</t>
+  </si>
+  <si>
+    <t>Ravi Ramawat</t>
+  </si>
+  <si>
+    <t>Jaipur</t>
   </si>
 </sst>
 </file>
@@ -646,12 +660,12 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="14.6328125" customWidth="1"/>
+    <col min="1" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -686,7 +700,7 @@
         <v>Below</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -704,7 +718,7 @@
         <v>Above</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -722,7 +736,7 @@
         <v>Above</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -740,7 +754,7 @@
         <v>Above</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -758,7 +772,7 @@
         <v>Above</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -770,7 +784,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -796,12 +810,12 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="14.6328125" customWidth="1"/>
+    <col min="1" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>40</v>
       </c>
@@ -824,7 +838,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>8</v>
       </c>
@@ -848,7 +862,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>7</v>
       </c>
@@ -872,7 +886,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>6</v>
       </c>
@@ -896,7 +910,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -920,7 +934,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -944,7 +958,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>SUM(A2:A6)</f>
         <v>30</v>
@@ -974,7 +988,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1002,37 +1016,37 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1050,16 +1064,16 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.81640625" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1079,7 +1093,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1099,7 +1113,7 @@
         <v>38022</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1119,7 +1133,7 @@
         <v>38024</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1139,7 +1153,7 @@
         <v>38027</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1159,7 +1173,7 @@
         <v>38029</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1179,7 +1193,7 @@
         <v>37998</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1199,7 +1213,7 @@
         <v>38001</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1242,47 +1256,47 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -1305,23 +1319,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF45558A-A75A-4821-B1B0-3240483A6336}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>